<commit_message>
updated XML and thesis
</commit_message>
<xml_diff>
--- a/pauses_data.xlsx
+++ b/pauses_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Documents\GitHub\Tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D9867BE-79C1-438D-945B-1E9B32DC8475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE0419-D552-43BD-BBA7-32244EA4B77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,10 +358,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
@@ -661,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2119,6 +2115,9 @@
       <c r="A91">
         <v>1</v>
       </c>
+      <c r="B91">
+        <v>1.6240000000000001E-2</v>
+      </c>
       <c r="D91" s="3">
         <f>(SUM(C91:C100))/10</f>
         <v>0</v>
@@ -2133,18 +2132,24 @@
       </c>
       <c r="G91">
         <f>COUNT(B91:B95)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2</v>
       </c>
+      <c r="B92">
+        <v>1.831E-2</v>
+      </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>3</v>
       </c>
+      <c r="B93">
+        <v>1.857E-2</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
@@ -2155,30 +2160,48 @@
       <c r="A95">
         <v>5</v>
       </c>
+      <c r="B95">
+        <v>2.8979999999999999E-2</v>
+      </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>6</v>
       </c>
+      <c r="B96">
+        <v>2.6339999999999999E-2</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7</v>
       </c>
+      <c r="B97">
+        <v>1.848E-2</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8</v>
       </c>
+      <c r="B98">
+        <v>4.4650000000000002E-2</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>9</v>
       </c>
+      <c r="B99">
+        <v>2.256E-2</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>10</v>
+      </c>
+      <c r="B100">
+        <v>2.4879999999999999E-2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2200,6 +2223,9 @@
       <c r="A102">
         <v>1</v>
       </c>
+      <c r="B102">
+        <v>1.9390000000000001E-2</v>
+      </c>
       <c r="D102" s="3">
         <f>(SUM(C102:C111))/10</f>
         <v>0</v>
@@ -2214,52 +2240,79 @@
       </c>
       <c r="G102">
         <f>COUNT(B102:B106)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2</v>
       </c>
+      <c r="B103">
+        <v>1.448E-2</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3</v>
       </c>
+      <c r="B104">
+        <v>2.0889999999999999E-2</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>4</v>
       </c>
+      <c r="B105">
+        <v>3.0779999999999998E-2</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>5</v>
       </c>
+      <c r="B106">
+        <v>3.0550000000000001E-2</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>6</v>
       </c>
+      <c r="B107">
+        <v>1.3780000000000001E-2</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7</v>
       </c>
+      <c r="B108">
+        <v>1.976E-2</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>8</v>
       </c>
+      <c r="B109">
+        <v>1.3140000000000001E-2</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>9</v>
       </c>
+      <c r="B110">
+        <v>2.4279999999999999E-2</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>10</v>
+      </c>
+      <c r="B111">
+        <v>2.579E-2</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -2616,6 +2669,9 @@
       <c r="A135">
         <v>1</v>
       </c>
+      <c r="B135">
+        <v>1.7160000000000002E-2</v>
+      </c>
       <c r="D135" s="3">
         <f>(SUM(C135:C144))/10</f>
         <v>0</v>
@@ -2630,52 +2686,79 @@
       </c>
       <c r="G135">
         <f>COUNT(B135:B139)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2</v>
       </c>
+      <c r="B136">
+        <v>5.1599999999999997E-3</v>
+      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>3</v>
       </c>
+      <c r="B137">
+        <v>1.298E-2</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>4</v>
       </c>
+      <c r="B138">
+        <v>1.321E-2</v>
+      </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>5</v>
       </c>
+      <c r="B139">
+        <v>1.485E-2</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6</v>
       </c>
+      <c r="B140">
+        <v>1.3270000000000001E-2</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>7</v>
       </c>
+      <c r="B141">
+        <v>1.554E-2</v>
+      </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>8</v>
       </c>
+      <c r="B142">
+        <v>1.384E-2</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>9</v>
       </c>
+      <c r="B143">
+        <v>9.7900000000000001E-3</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>10</v>
+      </c>
+      <c r="B144">
+        <v>2.7130000000000001E-2</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -2697,6 +2780,9 @@
       <c r="A146">
         <v>1</v>
       </c>
+      <c r="B146">
+        <v>1.524E-2</v>
+      </c>
       <c r="D146" s="3">
         <f>(SUM(C146:C155))/10</f>
         <v>0</v>
@@ -2711,52 +2797,79 @@
       </c>
       <c r="G146">
         <f>COUNT(B146:B150)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2</v>
       </c>
+      <c r="B147">
+        <v>9.1599999999999997E-3</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3</v>
       </c>
+      <c r="B148">
+        <v>1.068E-2</v>
+      </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>4</v>
       </c>
+      <c r="B149">
+        <v>2.3560000000000001E-2</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>5</v>
       </c>
+      <c r="B150">
+        <v>3.857E-2</v>
+      </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6</v>
       </c>
+      <c r="B151">
+        <v>1.0370000000000001E-2</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>7</v>
       </c>
+      <c r="B152">
+        <v>1.1509999999999999E-2</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>8</v>
       </c>
+      <c r="B153">
+        <v>1.089E-2</v>
+      </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>9</v>
       </c>
+      <c r="B154">
+        <v>7.8200000000000006E-3</v>
+      </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>10</v>
+      </c>
+      <c r="B155">
+        <v>2.239E-2</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -2889,6 +3002,9 @@
       <c r="A168">
         <v>1</v>
       </c>
+      <c r="B168">
+        <v>1.545E-2</v>
+      </c>
       <c r="D168" s="3">
         <f>(SUM(C168:C177))/10</f>
         <v>0</v>
@@ -2903,52 +3019,79 @@
       </c>
       <c r="G168">
         <f>COUNT(B168:B172)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2</v>
       </c>
+      <c r="B169">
+        <v>2.7019999999999999E-2</v>
+      </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>3</v>
       </c>
+      <c r="B170">
+        <v>1.115E-2</v>
+      </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>4</v>
       </c>
+      <c r="B171">
+        <v>1.18E-2</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>5</v>
       </c>
+      <c r="B172">
+        <v>1.357E-2</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>6</v>
       </c>
+      <c r="B173">
+        <v>8.4499999999999992E-3</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>7</v>
       </c>
+      <c r="B174">
+        <v>1.2149999999999999E-2</v>
+      </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>8</v>
       </c>
+      <c r="B175">
+        <v>1.008E-2</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>9</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>9.7300000000000008E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>10</v>
+      </c>
+      <c r="B177">
+        <v>2.2880000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added XML and finished code
</commit_message>
<xml_diff>
--- a/pauses_data.xlsx
+++ b/pauses_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Documents\GitHub\Tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE0419-D552-43BD-BBA7-32244EA4B77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1B7D53-B2BA-4349-BA1D-0041E8276016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
   <si>
     <t>RAW_VALUES</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>MAX</t>
-  </si>
-  <si>
-    <t>NUMBER</t>
   </si>
   <si>
     <t>P1</t>
@@ -103,15 +100,39 @@
   <si>
     <t>P7</t>
   </si>
+  <si>
+    <t>DEV.ST</t>
+  </si>
+  <si>
+    <t>AVG MALE</t>
+  </si>
+  <si>
+    <t>AVG FEMALE</t>
+  </si>
+  <si>
+    <t>DEV FEMALE</t>
+  </si>
+  <si>
+    <t>DEV MALE</t>
+  </si>
+  <si>
+    <t>MIN MALE</t>
+  </si>
+  <si>
+    <t>MIN FEMALE</t>
+  </si>
+  <si>
+    <t>MAX MALE</t>
+  </si>
+  <si>
+    <t>MAX FEMALE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[hh]\:mm\:ss"/>
-  </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -174,8 +195,14 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,12 +251,160 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -249,7 +424,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -259,8 +434,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Accent 1 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -655,18 +874,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N177"/>
+  <dimension ref="A1:Q177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="12.109375" customWidth="1"/>
+    <col min="1" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,37 +913,28 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -740,14 +958,36 @@
         <v>9.5380000000000003</v>
       </c>
       <c r="G3">
-        <f>COUNT(B14:B23)</f>
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <f>STDEV(C3:C12)</f>
+        <v>2.482839942037701</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -759,26 +999,17 @@
         <v>1.006</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="15"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -790,32 +1021,43 @@
         <v>2.2399999999999998</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="I5">
-        <f>D3</f>
-        <v>3.2282000000000002</v>
-      </c>
-      <c r="J5">
-        <f>E3</f>
-        <v>1.006</v>
-      </c>
-      <c r="K5">
-        <f>F3</f>
-        <v>9.5380000000000003</v>
-      </c>
-      <c r="L5">
-        <f>D14</f>
-        <v>2.7030000000000003</v>
-      </c>
-      <c r="M5">
-        <f>E14</f>
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="N5">
-        <f>F14</f>
-        <v>11.444000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="18">
+        <f>AVERAGE(D3,D47,D69,D157)</f>
+        <v>2.4501374999999999</v>
+      </c>
+      <c r="K5" s="19">
+        <f>AVERAGE(D25,D91,D113,D135)</f>
+        <v>1.9230499999999999</v>
+      </c>
+      <c r="L5" s="20">
+        <f>AVERAGE(G3,G47,G69,G157)</f>
+        <v>1.860077178332681</v>
+      </c>
+      <c r="M5" s="19">
+        <f>AVERAGE(G25,G91,G113,G135)</f>
+        <v>1.2495107022474143</v>
+      </c>
+      <c r="N5" s="20">
+        <f>AVERAGE(E3,E47,E69,E157)</f>
+        <v>0.74087499999999995</v>
+      </c>
+      <c r="O5" s="19">
+        <f>AVERAGE(E25,E91,E113,E135)</f>
+        <v>0.25174999999999997</v>
+      </c>
+      <c r="P5" s="18">
+        <f>AVERAGE(F3,F47,F69,F157)</f>
+        <v>7.2410000000000005</v>
+      </c>
+      <c r="Q5" s="19">
+        <f>AVERAGE(F25,F91,F113,F135)</f>
+        <v>4.319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -826,32 +1068,17 @@
         <f t="shared" si="0"/>
         <v>2.8610000000000002</v>
       </c>
-      <c r="I6">
-        <f>D47</f>
-        <v>0.98565000000000003</v>
-      </c>
-      <c r="J6">
-        <f>E47</f>
-        <v>0.55449999999999999</v>
-      </c>
-      <c r="K6">
-        <f>F47</f>
-        <v>1.522</v>
-      </c>
-      <c r="L6">
-        <f>D58</f>
-        <v>0.44669999999999999</v>
-      </c>
-      <c r="M6">
-        <f>E58</f>
-        <v>0.65200000000000002</v>
-      </c>
-      <c r="N6">
-        <f>F58</f>
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="15"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -862,16 +1089,43 @@
         <f t="shared" si="0"/>
         <v>1.294</v>
       </c>
-      <c r="I7">
-        <f>D69</f>
-        <v>3.2749999999999999</v>
-      </c>
-      <c r="L7">
-        <f>D80</f>
-        <v>2.9519000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="18">
+        <f>AVERAGE(D14,D58,D80,D168)</f>
+        <v>1.8239000000000001</v>
+      </c>
+      <c r="K7" s="19">
+        <f>AVERAGE(D36,D102,D124,D146)</f>
+        <v>1.3651250000000001</v>
+      </c>
+      <c r="L7" s="20">
+        <f>AVERAGE(G14,G58,G80,G168)</f>
+        <v>1.3837781405374432</v>
+      </c>
+      <c r="M7" s="19">
+        <f>AVERAGE(G36,G102,G124,G146)</f>
+        <v>0.56922076844901126</v>
+      </c>
+      <c r="N7" s="20">
+        <f>AVERAGE(E14,E58,E80,E168)</f>
+        <v>0.6120000000000001</v>
+      </c>
+      <c r="O7" s="19">
+        <f>AVERAGE(E36,E102,E124,E146)</f>
+        <v>0.67</v>
+      </c>
+      <c r="P7" s="18">
+        <f>AVERAGE(F14,F58,F80,F168)</f>
+        <v>5.1157500000000002</v>
+      </c>
+      <c r="Q7" s="19">
+        <f>AVERAGE(F36,F102,F124,F146)</f>
+        <v>2.5212500000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -882,8 +1136,12 @@
         <f t="shared" si="0"/>
         <v>2.2270000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -894,8 +1152,12 @@
         <f t="shared" si="0"/>
         <v>2.64</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -906,8 +1168,12 @@
         <f t="shared" si="0"/>
         <v>4.6920000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -918,8 +1184,12 @@
         <f t="shared" si="0"/>
         <v>3.9309999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -930,23 +1200,31 @@
         <f t="shared" si="0"/>
         <v>9.5380000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -970,11 +1248,11 @@
         <v>11.444000000000001</v>
       </c>
       <c r="G14">
-        <f>COUNT(B14:B23)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <f>STDEV(C14:C23)</f>
+        <v>3.2764511628013357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -986,7 +1264,7 @@
         <v>0.52400000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1076,7 +1354,7 @@
       <c r="A23">
         <v>10</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>0.11444</v>
       </c>
       <c r="C23">
@@ -1086,13 +1364,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1123,8 +1401,8 @@
         <v>1.3080000000000001</v>
       </c>
       <c r="G25">
-        <f>COUNT(B25:B34)</f>
-        <v>10</v>
+        <f>STDEV(C25:C34)</f>
+        <v>0.26213484655378755</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1153,7 +1431,7 @@
       </c>
       <c r="D27" s="4"/>
       <c r="H27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,7 +1506,7 @@
         <v>1.1169999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1243,7 +1521,7 @@
         <v>2.0580000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1258,22 +1536,22 @@
         <v>1.457E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1297,11 +1575,11 @@
         <v>1.0009999999999999</v>
       </c>
       <c r="G36">
-        <f>COUNT(B36:B45)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <f>STDEV(C36:C45)</f>
+        <v>0.18797635785148945</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1314,7 +1592,7 @@
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1327,7 +1605,7 @@
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1339,7 +1617,7 @@
         <v>0.79699999999999993</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1351,7 +1629,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1363,7 +1641,7 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1375,7 +1653,7 @@
         <v>0.58399999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8</v>
       </c>
@@ -1390,7 +1668,7 @@
         <v>1.506E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -1405,7 +1683,7 @@
         <v>1.3050000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>10</v>
       </c>
@@ -1419,26 +1697,23 @@
       <c r="H45">
         <v>1.1339999999999999E-2</v>
       </c>
-      <c r="I45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1462,14 +1737,14 @@
         <v>1.522</v>
       </c>
       <c r="G47">
-        <f>COUNT(#REF!)</f>
-        <v>0</v>
+        <f>STDEV(C47:C56)</f>
+        <v>0.2966915766695557</v>
       </c>
       <c r="H47">
         <v>1.4069999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1481,7 +1756,7 @@
         <v>0.89200000000000013</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1496,7 +1771,7 @@
         <v>1.183E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -1508,11 +1783,11 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="5">
         <v>9.0200000000000002E-3</v>
       </c>
       <c r="C51">
@@ -1522,11 +1797,8 @@
       <c r="H51">
         <v>1.7919999999999998E-2</v>
       </c>
-      <c r="I51" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -1541,7 +1813,7 @@
         <v>1.9480000000000001E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7</v>
       </c>
@@ -1556,7 +1828,7 @@
         <v>2.5090000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
@@ -1571,7 +1843,7 @@
         <v>4.2509999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9</v>
       </c>
@@ -1586,7 +1858,7 @@
         <v>5.1040000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>10</v>
       </c>
@@ -1601,22 +1873,22 @@
         <v>4.2450000000000002E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1640,14 +1912,14 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="G58">
-        <f>COUNT(B58:B62)</f>
-        <v>5</v>
+        <f>STDEV(C58:C67)</f>
+        <v>0.26933137375524802</v>
       </c>
       <c r="H58">
         <v>1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1662,7 +1934,7 @@
         <v>1.069E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1677,7 +1949,7 @@
         <v>2.7449999999999999E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -1692,7 +1964,7 @@
         <v>3.5090000000000003E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5</v>
       </c>
@@ -1704,7 +1976,7 @@
         <v>0.97400000000000009</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>6</v>
       </c>
@@ -1716,7 +1988,7 @@
         <v>0.70200000000000007</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7</v>
       </c>
@@ -1728,7 +2000,7 @@
         <v>0.68799999999999994</v>
       </c>
       <c r="F64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H64">
         <v>2.7E-2</v>
@@ -1775,13 +2047,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -1812,8 +2084,8 @@
         <v>8.4239999999999995</v>
       </c>
       <c r="G69">
-        <f>COUNT(B69:B78)</f>
-        <v>10</v>
+        <f>STDEV(C69:C78)</f>
+        <v>1.9948358328443976</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,7 +2166,7 @@
         <v>2.5829999999999997</v>
       </c>
       <c r="F75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -1938,13 +2210,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -1975,8 +2247,8 @@
         <v>5.1669999999999998</v>
       </c>
       <c r="G80">
-        <f>COUNT(B80:B84)</f>
-        <v>5</v>
+        <f>STDEV(C80:C89)</f>
+        <v>1.317550795984731</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,7 +2287,7 @@
         <v>1.7909999999999999</v>
       </c>
       <c r="K83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2054,7 +2326,7 @@
         <v>1.907</v>
       </c>
       <c r="F86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -2098,13 +2370,13 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -2118,9 +2390,13 @@
       <c r="B91">
         <v>1.6240000000000001E-2</v>
       </c>
+      <c r="C91">
+        <f>B96*100</f>
+        <v>2.6339999999999999</v>
+      </c>
       <c r="D91" s="3">
         <f>(SUM(C91:C100))/10</f>
-        <v>0</v>
+        <v>2.1901000000000002</v>
       </c>
       <c r="E91" s="3">
         <f>MIN(C91:C100)</f>
@@ -2128,11 +2404,11 @@
       </c>
       <c r="F91" s="3">
         <f>MAX(C91:C100)</f>
-        <v>0</v>
+        <v>4.4649999999999999</v>
       </c>
       <c r="G91">
-        <f>COUNT(B91:B95)</f>
-        <v>4</v>
+        <f>STDEV(C91:C100)</f>
+        <v>1.1274541084526095</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -2142,6 +2418,10 @@
       <c r="B92">
         <v>1.831E-2</v>
       </c>
+      <c r="C92">
+        <f>B97*100</f>
+        <v>1.8480000000000001</v>
+      </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -2150,11 +2430,19 @@
       <c r="B93">
         <v>1.857E-2</v>
       </c>
+      <c r="C93">
+        <f>B98*100</f>
+        <v>4.4649999999999999</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4</v>
       </c>
+      <c r="C94">
+        <f>B99*100</f>
+        <v>2.2560000000000002</v>
+      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
@@ -2163,6 +2451,10 @@
       <c r="B95">
         <v>2.8979999999999999E-2</v>
       </c>
+      <c r="C95">
+        <f>B100*100</f>
+        <v>2.488</v>
+      </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
@@ -2171,6 +2463,10 @@
       <c r="B96">
         <v>2.6339999999999999E-2</v>
       </c>
+      <c r="C96">
+        <f>B91*100</f>
+        <v>1.6240000000000001</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -2179,6 +2475,10 @@
       <c r="B97">
         <v>1.848E-2</v>
       </c>
+      <c r="C97">
+        <f>B92*100</f>
+        <v>1.831</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
@@ -2187,6 +2487,10 @@
       <c r="B98">
         <v>4.4650000000000002E-2</v>
       </c>
+      <c r="C98">
+        <f>B93*100</f>
+        <v>1.857</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
@@ -2195,6 +2499,10 @@
       <c r="B99">
         <v>2.256E-2</v>
       </c>
+      <c r="C99">
+        <f>B94*100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -2203,16 +2511,20 @@
       <c r="B100">
         <v>2.4879999999999999E-2</v>
       </c>
+      <c r="C100">
+        <f>B95*100</f>
+        <v>2.8979999999999997</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -2226,21 +2538,25 @@
       <c r="B102">
         <v>1.9390000000000001E-2</v>
       </c>
+      <c r="C102">
+        <f>B107*100</f>
+        <v>1.3780000000000001</v>
+      </c>
       <c r="D102" s="3">
         <f>(SUM(C102:C111))/10</f>
-        <v>0</v>
+        <v>2.1284000000000001</v>
       </c>
       <c r="E102" s="3">
         <f>MIN(C102:C111)</f>
-        <v>0</v>
+        <v>1.3140000000000001</v>
       </c>
       <c r="F102" s="3">
         <f>MAX(C102:C111)</f>
-        <v>0</v>
+        <v>3.0779999999999998</v>
       </c>
       <c r="G102">
-        <f>COUNT(B102:B106)</f>
-        <v>5</v>
+        <f>STDEV(C102:C111)</f>
+        <v>0.65004875030860299</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -2250,6 +2566,10 @@
       <c r="B103">
         <v>1.448E-2</v>
       </c>
+      <c r="C103">
+        <f>B108*100</f>
+        <v>1.976</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -2258,6 +2578,10 @@
       <c r="B104">
         <v>2.0889999999999999E-2</v>
       </c>
+      <c r="C104">
+        <f>B109*100</f>
+        <v>1.3140000000000001</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -2266,6 +2590,10 @@
       <c r="B105">
         <v>3.0779999999999998E-2</v>
       </c>
+      <c r="C105">
+        <f>B110*100</f>
+        <v>2.4279999999999999</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -2274,6 +2602,10 @@
       <c r="B106">
         <v>3.0550000000000001E-2</v>
       </c>
+      <c r="C106">
+        <f>B111*100</f>
+        <v>2.5790000000000002</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -2282,6 +2614,10 @@
       <c r="B107">
         <v>1.3780000000000001E-2</v>
       </c>
+      <c r="C107">
+        <f>B102*100</f>
+        <v>1.9390000000000001</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
@@ -2290,6 +2626,10 @@
       <c r="B108">
         <v>1.976E-2</v>
       </c>
+      <c r="C108">
+        <f>B103*100</f>
+        <v>1.448</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
@@ -2298,6 +2638,10 @@
       <c r="B109">
         <v>1.3140000000000001E-2</v>
       </c>
+      <c r="C109">
+        <f>B104*100</f>
+        <v>2.089</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
@@ -2306,6 +2650,10 @@
       <c r="B110">
         <v>2.4279999999999999E-2</v>
       </c>
+      <c r="C110">
+        <f>B105*100</f>
+        <v>3.0779999999999998</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -2314,16 +2662,20 @@
       <c r="B111">
         <v>2.579E-2</v>
       </c>
+      <c r="C111">
+        <f>B106*100</f>
+        <v>3.0550000000000002</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -2354,8 +2706,8 @@
         <v>9.786999999999999</v>
       </c>
       <c r="G113">
-        <f>COUNT(A113:A122)</f>
-        <v>10</v>
+        <f>STDEV(C113:C122)</f>
+        <v>3.08287649949055</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -2445,7 +2797,7 @@
         <v>2.5829999999999997</v>
       </c>
       <c r="F119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H119">
         <v>4.0620000000000003E-2</v>
@@ -2492,13 +2844,13 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -2529,8 +2881,8 @@
         <v>2.149</v>
       </c>
       <c r="G124">
-        <f>COUNT(B124:B128)</f>
-        <v>5</v>
+        <f>STDEV(C124:C133)</f>
+        <v>0.38802676024556165</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -2605,7 +2957,7 @@
         <v>0.99199999999999999</v>
       </c>
       <c r="F130" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H130">
         <v>0.20380000000000001</v>
@@ -2652,13 +3004,13 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -2672,9 +3024,13 @@
       <c r="B135">
         <v>1.7160000000000002E-2</v>
       </c>
+      <c r="C135">
+        <f>B140*100</f>
+        <v>1.327</v>
+      </c>
       <c r="D135" s="3">
         <f>(SUM(C135:C144))/10</f>
-        <v>0</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="E135" s="3">
         <f>MIN(C135:C144)</f>
@@ -2682,11 +3038,11 @@
       </c>
       <c r="F135" s="3">
         <f>MAX(C135:C144)</f>
-        <v>0</v>
+        <v>1.7160000000000002</v>
       </c>
       <c r="G135">
-        <f>COUNT(B135:B139)</f>
-        <v>5</v>
+        <f>STDEV(C135:C144)</f>
+        <v>0.52557735449270993</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,6 +3052,10 @@
       <c r="B136">
         <v>5.1599999999999997E-3</v>
       </c>
+      <c r="C136">
+        <f>B141*100</f>
+        <v>1.554</v>
+      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -2704,6 +3064,10 @@
       <c r="B137">
         <v>1.298E-2</v>
       </c>
+      <c r="C137">
+        <f>B142*100</f>
+        <v>1.3839999999999999</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
@@ -2712,6 +3076,10 @@
       <c r="B138">
         <v>1.321E-2</v>
       </c>
+      <c r="C138">
+        <f>B143*100</f>
+        <v>0.97899999999999998</v>
+      </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
@@ -2720,6 +3088,10 @@
       <c r="B139">
         <v>1.485E-2</v>
       </c>
+      <c r="C139">
+        <f>H144*100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -2728,6 +3100,10 @@
       <c r="B140">
         <v>1.3270000000000001E-2</v>
       </c>
+      <c r="C140">
+        <f>B135*100</f>
+        <v>1.7160000000000002</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
@@ -2736,6 +3112,10 @@
       <c r="B141">
         <v>1.554E-2</v>
       </c>
+      <c r="C141">
+        <f>B136*100</f>
+        <v>0.51600000000000001</v>
+      </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -2744,6 +3124,10 @@
       <c r="B142">
         <v>1.384E-2</v>
       </c>
+      <c r="C142">
+        <f>B137*100</f>
+        <v>1.298</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
@@ -2752,6 +3136,10 @@
       <c r="B143">
         <v>9.7900000000000001E-3</v>
       </c>
+      <c r="C143">
+        <f>B138*100</f>
+        <v>1.321</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -2760,32 +3148,40 @@
       <c r="B144">
         <v>2.7130000000000001E-2</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <f>B139*100</f>
+        <v>1.4850000000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1</v>
       </c>
       <c r="B146">
         <v>1.524E-2</v>
       </c>
+      <c r="C146">
+        <f>B151*100</f>
+        <v>1.0370000000000001</v>
+      </c>
       <c r="D146" s="3">
         <f>(SUM(C146:C155))/10</f>
-        <v>0</v>
+        <v>1.3780000000000001</v>
       </c>
       <c r="E146" s="3">
         <f>MIN(C146:C155)</f>
@@ -2793,110 +3189,152 @@
       </c>
       <c r="F146" s="3">
         <f>MAX(C146:C155)</f>
-        <v>0</v>
+        <v>3.8570000000000002</v>
       </c>
       <c r="G146">
-        <f>COUNT(B146:B150)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+        <f>STDEV(C146:C155)</f>
+        <v>1.050831205390391</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2</v>
       </c>
       <c r="B147">
         <v>9.1599999999999997E-3</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <f>B152*100</f>
+        <v>1.151</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3</v>
       </c>
       <c r="B148">
         <v>1.068E-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <f>B153*100</f>
+        <v>1.089</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>4</v>
       </c>
       <c r="B149">
         <v>2.3560000000000001E-2</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <f>B154*100</f>
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>5</v>
       </c>
       <c r="B150">
         <v>3.857E-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <f>I155*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6</v>
       </c>
       <c r="B151">
         <v>1.0370000000000001E-2</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <f>B146*100</f>
+        <v>1.524</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>7</v>
       </c>
       <c r="B152">
         <v>1.1509999999999999E-2</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <f>B147*100</f>
+        <v>0.91599999999999993</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>8</v>
       </c>
       <c r="B153">
         <v>1.089E-2</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <f>B148*100</f>
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="H153" s="7"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>9</v>
       </c>
       <c r="B154">
         <v>7.8200000000000006E-3</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <f>B149*100</f>
+        <v>2.3560000000000003</v>
+      </c>
+      <c r="H154" s="7"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>10</v>
       </c>
       <c r="B155">
         <v>2.239E-2</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <f>B150*100</f>
+        <v>3.8570000000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B156" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1</v>
       </c>
       <c r="B157">
         <v>8.8999999999999999E-3</v>
       </c>
+      <c r="C157">
+        <f>B162*100</f>
+        <v>1.4970000000000001</v>
+      </c>
       <c r="D157" s="3">
         <f>(SUM(C157:C166))/10</f>
-        <v>0</v>
+        <v>2.3117000000000005</v>
       </c>
       <c r="E157" s="3">
         <f>MIN(C157:C166)</f>
@@ -2904,35 +3342,47 @@
       </c>
       <c r="F157" s="3">
         <f>MAX(C157:C166)</f>
-        <v>0</v>
+        <v>9.48</v>
       </c>
       <c r="G157">
-        <f>COUNT(B157:B161)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+        <f>STDEV(C157:C166)</f>
+        <v>2.6659413617790704</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2</v>
       </c>
       <c r="B158">
         <v>2.5080000000000002E-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <f>B163*100</f>
+        <v>1.1060000000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>3</v>
       </c>
       <c r="B159">
         <v>1.4189999999999999E-2</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <f>B164*100</f>
+        <v>3.2359999999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>4</v>
       </c>
       <c r="B160">
         <v>1.3180000000000001E-2</v>
+      </c>
+      <c r="C160">
+        <f>B165*100</f>
+        <v>1.6629999999999998</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,6 +3392,10 @@
       <c r="B161">
         <v>9.4799999999999995E-2</v>
       </c>
+      <c r="C161">
+        <f>I166*100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
@@ -2950,6 +3404,10 @@
       <c r="B162">
         <v>1.4970000000000001E-2</v>
       </c>
+      <c r="C162">
+        <f>B157*100</f>
+        <v>0.89</v>
+      </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
@@ -2958,6 +3416,10 @@
       <c r="B163">
         <v>1.106E-2</v>
       </c>
+      <c r="C163">
+        <f>B158*100</f>
+        <v>2.508</v>
+      </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
@@ -2966,6 +3428,10 @@
       <c r="B164">
         <v>3.236E-2</v>
       </c>
+      <c r="C164">
+        <f>B159*100</f>
+        <v>1.419</v>
+      </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
@@ -2974,6 +3440,10 @@
       <c r="B165">
         <v>1.6629999999999999E-2</v>
       </c>
+      <c r="C165">
+        <f>B160*100</f>
+        <v>1.3180000000000001</v>
+      </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
@@ -2982,16 +3452,20 @@
       <c r="B166">
         <v>2.3120000000000002E-2</v>
       </c>
+      <c r="C166">
+        <f>B161*100</f>
+        <v>9.48</v>
+      </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -3005,9 +3479,13 @@
       <c r="B168">
         <v>1.545E-2</v>
       </c>
+      <c r="C168">
+        <f>B173*100</f>
+        <v>0.84499999999999997</v>
+      </c>
       <c r="D168" s="3">
         <f>(SUM(C168:C177))/10</f>
-        <v>0</v>
+        <v>1.194</v>
       </c>
       <c r="E168" s="3">
         <f>MIN(C168:C177)</f>
@@ -3015,11 +3493,11 @@
       </c>
       <c r="F168" s="3">
         <f>MAX(C168:C177)</f>
-        <v>0</v>
+        <v>2.702</v>
       </c>
       <c r="G168">
-        <f>COUNT(B168:B172)</f>
-        <v>5</v>
+        <f>STDEV(C168:C177)</f>
+        <v>0.67177922960845815</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -3029,6 +3507,10 @@
       <c r="B169">
         <v>2.7019999999999999E-2</v>
       </c>
+      <c r="C169">
+        <f>B174*100</f>
+        <v>1.2149999999999999</v>
+      </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
@@ -3037,6 +3519,10 @@
       <c r="B170">
         <v>1.115E-2</v>
       </c>
+      <c r="C170">
+        <f>B175*100</f>
+        <v>1.008</v>
+      </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
@@ -3045,6 +3531,10 @@
       <c r="B171">
         <v>1.18E-2</v>
       </c>
+      <c r="C171">
+        <f>B176*100</f>
+        <v>0.97300000000000009</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
@@ -3053,6 +3543,10 @@
       <c r="B172">
         <v>1.357E-2</v>
       </c>
+      <c r="C172">
+        <f>H177*100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
@@ -3061,6 +3555,10 @@
       <c r="B173">
         <v>8.4499999999999992E-3</v>
       </c>
+      <c r="C173">
+        <f>B168*100</f>
+        <v>1.5449999999999999</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
@@ -3069,6 +3567,10 @@
       <c r="B174">
         <v>1.2149999999999999E-2</v>
       </c>
+      <c r="C174">
+        <f>B169*100</f>
+        <v>2.702</v>
+      </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
@@ -3077,6 +3579,10 @@
       <c r="B175">
         <v>1.008E-2</v>
       </c>
+      <c r="C175">
+        <f>B170*100</f>
+        <v>1.115</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
@@ -3085,13 +3591,21 @@
       <c r="B176">
         <v>9.7300000000000008E-3</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176">
+        <f>B171*100</f>
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>10</v>
       </c>
       <c r="B177">
         <v>2.2880000000000001E-2</v>
+      </c>
+      <c r="C177">
+        <f>B172*100</f>
+        <v>1.357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>